<commit_message>
feat: nuovi test case validazione
</commit_message>
<xml_diff>
--- a/Test Case/Validazione/1-Referto di Radiologia/CDA2_Referto_di_Radiologia_KO.xlsx
+++ b/Test Case/Validazione/1-Referto di Radiologia/CDA2_Referto_di_Radiologia_KO.xlsx
@@ -75547,13 +75547,17 @@
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d04b37e-0497-498c-96f6-8855740e5edb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099D50BAF6148C0469FC2106F96A8440B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0c25bf1fc3184a9914f412ea273c11a4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d04b37e-0497-498c-96f6-8855740e5edb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88da7026946f39f8a400a0307dada779" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099D50BAF6148C0469FC2106F96A8440B" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7768c764893153760d939b2a04face0b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d04b37e-0497-498c-96f6-8855740e5edb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ef69b4f9d45f678c0f7c9c89f8623db" ns2:_="">
     <xsd:import namespace="3d04b37e-0497-498c-96f6-8855740e5edb"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -75565,6 +75569,10 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -75593,6 +75601,30 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="33ef62f9-2e07-484b-bd79-00aec90129fe" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -75720,19 +75752,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1ADBF96-0AD3-4F24-956B-1BB331964E0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3d04b37e-0497-498c-96f6-8855740e5edb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4496047E-5714-42AC-93F0-1C3354B4CB73}"/>
 </file>
</xml_diff>

<commit_message>
nuovi test case validazione
</commit_message>
<xml_diff>
--- a/Test Case/Validazione/1-Referto di Radiologia/CDA2_Referto_di_Radiologia_KO.xlsx
+++ b/Test Case/Validazione/1-Referto di Radiologia/CDA2_Referto_di_Radiologia_KO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://people.ey.com/personal/ludovica_luciani_it_ey_com/Documents/Desktop/[Accreditamento_Fornitori] - Casi d'uso OK &amp; KO - consegna finale/1-Referto di Radiologia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sites.ey.com/sites/IBM-SOGEI-Sogei-FSE2.0-GTW/Shared Documents/Sogei - FSE 2.0 - GTW/02.  Accreditamento - contributo SME per checklist/Validazione/[Accreditamento_Fornitori] - TC OK &amp; KO - 20231213/1-Referto di Radiologia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{1B3E985C-6B62-4DD6-A184-B79E80055DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAAE3101-3CE4-4CA7-B013-847936E9E7BC}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{1B3E985C-6B62-4DD6-A184-B79E80055DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1523741B-BDD5-4CD7-8276-7003396D9276}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="802" firstSheet="14" activeTab="20" xr2:uid="{1E8B7D17-95DA-407D-AD12-13C95143136E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="802" activeTab="2" xr2:uid="{1E8B7D17-95DA-407D-AD12-13C95143136E}"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDA" sheetId="17" r:id="rId1"/>
@@ -3352,9 +3352,6 @@
     <t>Non è presente l'elemento che riporta l'identificativo della prescrizione</t>
   </si>
   <si>
-    <t>Valorizzazione errata del codice fiscale con caratteri in minuscolo e con un numero inferiore di 16 caratteri (es:  "PROVAX00x00x0x")</t>
-  </si>
-  <si>
     <t>L'elemento viene valorizzato erroneamente con un livello di riservatezza moderatamente sensibile ("Restricted")</t>
   </si>
   <si>
@@ -3374,6 +3371,9 @@
   </si>
   <si>
     <t>Viene inserita una diagnosi al quale è associato un codice errato, che non appartiene al sistema di codifica utilizzato (ICD-9-CM).</t>
+  </si>
+  <si>
+    <t>Valorizzazione errata del codice fiscale con caratteri in minuscolo (es:  "provax00x00x000x")</t>
   </si>
 </sst>
 </file>
@@ -4873,7 +4873,7 @@
   <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11834,7 +11834,7 @@
         <v>976</v>
       </c>
       <c r="F210" s="106" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="211" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -34313,7 +34313,7 @@
         <v>827</v>
       </c>
       <c r="F141" s="106" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -40704,7 +40704,7 @@
         <v>617</v>
       </c>
       <c r="F43" s="122" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -43935,7 +43935,7 @@
   <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="E28" sqref="E28:E32"/>
@@ -47512,7 +47512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68F7FA9-4ADF-4973-959A-F35DA51D94BD}">
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="40" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E163" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -51022,11 +51022,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E51970-45E7-423A-A6F9-1C957942FC2A}">
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E43" sqref="E43:E46"/>
+      <selection pane="bottomRight" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51727,7 +51727,7 @@
         <v>116</v>
       </c>
       <c r="E43" s="98" t="s">
-        <v>1055</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -54991,7 +54991,7 @@
         <v>79</v>
       </c>
       <c r="E28" s="101" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -58869,7 +58869,7 @@
         <v>135</v>
       </c>
       <c r="E52" s="58" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -61530,7 +61530,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E62" sqref="E62"/>
+      <selection pane="bottomRight" activeCell="D62" sqref="D62:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -66039,7 +66039,7 @@
         <v>159</v>
       </c>
       <c r="E63" s="98" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -68534,7 +68534,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E143" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A155" sqref="A155"/>
+      <selection pane="bottomRight" activeCell="E144" sqref="E144:E148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70816,7 +70816,7 @@
         <v>329</v>
       </c>
       <c r="E144" s="98" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -75537,28 +75537,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d04b37e-0497-498c-96f6-8855740e5edb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099D50BAF6148C0469FC2106F96A8440B" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7768c764893153760d939b2a04face0b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d04b37e-0497-498c-96f6-8855740e5edb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ef69b4f9d45f678c0f7c9c89f8623db" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010099D50BAF6148C0469FC2106F96A8440B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40ae23d0b881bcbe4284a7303aad900d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d04b37e-0497-498c-96f6-8855740e5edb" xmlns:ns3="14722739-9480-433a-8c7c-4ec5d8a77ba5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="65be93e378bc8cf519a145410d46ce17" ns2:_="" ns3:_="">
     <xsd:import namespace="3d04b37e-0497-498c-96f6-8855740e5edb"/>
+    <xsd:import namespace="14722739-9480-433a-8c7c-4ec5d8a77ba5"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -75573,6 +75555,10 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -75625,6 +75611,46 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="17" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="18" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="14722739-9480-433a-8c7c-4ec5d8a77ba5" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -75727,10 +75753,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d04b37e-0497-498c-96f6-8855740e5edb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51A983D-5463-4E4A-8B75-1C405A420DB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2342556D-47EE-4215-8B11-1DDC3F91AB91}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3d04b37e-0497-498c-96f6-8855740e5edb"/>
+    <ds:schemaRef ds:uri="14722739-9480-433a-8c7c-4ec5d8a77ba5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -75738,19 +75794,24 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C0AEB7-C55A-461D-A0CE-4337A3223303}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="14722739-9480-433a-8c7c-4ec5d8a77ba5"/>
+    <ds:schemaRef ds:uri="3d04b37e-0497-498c-96f6-8855740e5edb"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3d04b37e-0497-498c-96f6-8855740e5edb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4496047E-5714-42AC-93F0-1C3354B4CB73}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51A983D-5463-4E4A-8B75-1C405A420DB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiornamento documentazione per RAD
</commit_message>
<xml_diff>
--- a/Test Case/Validazione/1-Referto di Radiologia/CDA2_Referto_di_Radiologia_KO.xlsx
+++ b/Test Case/Validazione/1-Referto di Radiologia/CDA2_Referto_di_Radiologia_KO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sites.ey.com/sites/IBM-SOGEI-Sogei-FSE2.0-GTW/Shared Documents/Sogei - FSE 2.0 - GTW/02.  Accreditamento - contributo SME per checklist/Validazione/[Accreditamento_Fornitori] - TC OK &amp; KO - 20231213/1-Referto di Radiologia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AF833DV\Downloads\1-Referto di Radiologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{1B3E985C-6B62-4DD6-A184-B79E80055DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1523741B-BDD5-4CD7-8276-7003396D9276}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF2BEEA-D945-4D07-9458-4AF9B5465CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="802" activeTab="2" xr2:uid="{1E8B7D17-95DA-407D-AD12-13C95143136E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="802" activeTab="1" xr2:uid="{1E8B7D17-95DA-407D-AD12-13C95143136E}"/>
   </bookViews>
   <sheets>
     <sheet name="LEGENDA" sheetId="17" r:id="rId1"/>
@@ -3878,7 +3878,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -4131,12 +4131,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4574,9 +4568,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4614,7 +4608,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4720,7 +4714,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4862,7 +4856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7410,7 +7404,7 @@
       <c r="D158" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="E158" s="106" t="s">
+      <c r="E158" s="104" t="s">
         <v>1054</v>
       </c>
     </row>
@@ -7427,7 +7421,7 @@
       <c r="D159" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="E159" s="107"/>
+      <c r="E159" s="105"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="88" t="s">
@@ -7442,7 +7436,7 @@
       <c r="D160" s="28" t="s">
         <v>376</v>
       </c>
-      <c r="E160" s="107"/>
+      <c r="E160" s="105"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="27" t="s">
@@ -7457,7 +7451,7 @@
       <c r="D161" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="E161" s="108"/>
+      <c r="E161" s="106"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="63" t="s">
@@ -7472,7 +7466,7 @@
       <c r="D162" s="64" t="s">
         <v>379</v>
       </c>
-      <c r="E162" s="95"/>
+      <c r="E162" s="93"/>
     </row>
     <row r="163" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A163" s="63" t="s">
@@ -7487,7 +7481,7 @@
       <c r="D163" s="64" t="s">
         <v>525</v>
       </c>
-      <c r="E163" s="96"/>
+      <c r="E163" s="94"/>
     </row>
     <row r="164" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A164" s="63" t="s">
@@ -7502,7 +7496,7 @@
       <c r="D164" s="64" t="s">
         <v>526</v>
       </c>
-      <c r="E164" s="96"/>
+      <c r="E164" s="94"/>
     </row>
     <row r="165" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="63" t="s">
@@ -7517,7 +7511,7 @@
       <c r="D165" s="64" t="s">
         <v>387</v>
       </c>
-      <c r="E165" s="96"/>
+      <c r="E165" s="94"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="63" t="s">
@@ -7532,7 +7526,7 @@
       <c r="D166" s="64" t="s">
         <v>390</v>
       </c>
-      <c r="E166" s="97"/>
+      <c r="E166" s="95"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="20" t="s">
@@ -11833,7 +11827,7 @@
       <c r="E210" s="12" t="s">
         <v>976</v>
       </c>
-      <c r="F210" s="106" t="s">
+      <c r="F210" s="104" t="s">
         <v>1059</v>
       </c>
     </row>
@@ -11850,7 +11844,7 @@
       <c r="E211" s="12" t="s">
         <v>978</v>
       </c>
-      <c r="F211" s="107"/>
+      <c r="F211" s="105"/>
     </row>
     <row r="212" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B212" s="11" t="s">
@@ -11865,7 +11859,7 @@
       <c r="E212" s="12" t="s">
         <v>980</v>
       </c>
-      <c r="F212" s="107"/>
+      <c r="F212" s="105"/>
     </row>
     <row r="213" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B213" s="11" t="s">
@@ -11880,7 +11874,7 @@
       <c r="E213" s="12" t="s">
         <v>982</v>
       </c>
-      <c r="F213" s="107"/>
+      <c r="F213" s="105"/>
     </row>
     <row r="214" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B214" s="11" t="s">
@@ -11895,7 +11889,7 @@
       <c r="E214" s="12" t="s">
         <v>984</v>
       </c>
-      <c r="F214" s="108"/>
+      <c r="F214" s="106"/>
     </row>
     <row r="215" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B215" s="40" t="s">
@@ -12571,7 +12565,7 @@
       <c r="E11" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="1:24" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="70"/>
@@ -12587,7 +12581,7 @@
       <c r="E12" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="70"/>
@@ -12603,7 +12597,7 @@
       <c r="E13" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="70"/>
@@ -12619,7 +12613,7 @@
       <c r="E14" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="110"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="70"/>
@@ -12635,7 +12629,7 @@
       <c r="E15" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="110"/>
+      <c r="F15" s="108"/>
     </row>
     <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="70"/>
@@ -12651,7 +12645,7 @@
       <c r="E16" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="108"/>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="70"/>
@@ -12667,7 +12661,7 @@
       <c r="E17" s="72" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="70"/>
@@ -12683,7 +12677,7 @@
       <c r="E18" s="72" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="70"/>
@@ -12699,7 +12693,7 @@
       <c r="E19" s="72" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="110"/>
+      <c r="F19" s="108"/>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="70"/>
@@ -12715,7 +12709,7 @@
       <c r="E20" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="110"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="70"/>
@@ -12731,7 +12725,7 @@
       <c r="E21" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="70"/>
@@ -12747,7 +12741,7 @@
       <c r="E22" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="70"/>
@@ -12763,7 +12757,7 @@
       <c r="E23" s="72" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="110"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="70"/>
@@ -12779,7 +12773,7 @@
       <c r="E24" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="110"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="70"/>
@@ -12795,7 +12789,7 @@
       <c r="E25" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="111"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="40" t="s">
@@ -14651,7 +14645,7 @@
       <c r="E141" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="109"/>
+      <c r="F141" s="107"/>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B142" s="71" t="s">
@@ -14666,7 +14660,7 @@
       <c r="E142" s="72" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="112"/>
+      <c r="F142" s="110"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="71" t="s">
@@ -14681,7 +14675,7 @@
       <c r="E143" s="72" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="113"/>
+      <c r="F143" s="111"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="40" t="s">
@@ -15917,7 +15911,7 @@
       <c r="E219" s="12" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="106" t="s">
+      <c r="F219" s="104" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -15934,7 +15928,7 @@
       <c r="E220" s="12" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="107"/>
+      <c r="F220" s="105"/>
     </row>
     <row r="221" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B221" s="11" t="s">
@@ -15949,7 +15943,7 @@
       <c r="E221" s="12" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="107"/>
+      <c r="F221" s="105"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="11" t="s">
@@ -15964,7 +15958,7 @@
       <c r="E222" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="107"/>
+      <c r="F222" s="105"/>
     </row>
     <row r="223" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="11" t="s">
@@ -15979,7 +15973,7 @@
       <c r="E223" s="12" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="107"/>
+      <c r="F223" s="105"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="11" t="s">
@@ -15994,7 +15988,7 @@
       <c r="E224" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="107"/>
+      <c r="F224" s="105"/>
     </row>
     <row r="225" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B225" s="11" t="s">
@@ -16009,7 +16003,7 @@
       <c r="E225" s="12" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="107"/>
+      <c r="F225" s="105"/>
     </row>
     <row r="226" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B226" s="11" t="s">
@@ -16024,7 +16018,7 @@
       <c r="E226" s="12" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="108"/>
+      <c r="F226" s="106"/>
     </row>
     <row r="227" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B227" s="40" t="s">
@@ -16512,7 +16506,7 @@
       <c r="E11" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="1:24" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="70"/>
@@ -16528,7 +16522,7 @@
       <c r="E12" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="70"/>
@@ -16544,7 +16538,7 @@
       <c r="E13" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="70"/>
@@ -16560,7 +16554,7 @@
       <c r="E14" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="110"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="70"/>
@@ -16576,7 +16570,7 @@
       <c r="E15" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="110"/>
+      <c r="F15" s="108"/>
     </row>
     <row r="16" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="70"/>
@@ -16592,7 +16586,7 @@
       <c r="E16" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="108"/>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="70"/>
@@ -16608,7 +16602,7 @@
       <c r="E17" s="72" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="70"/>
@@ -16624,7 +16618,7 @@
       <c r="E18" s="72" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="70"/>
@@ -16640,7 +16634,7 @@
       <c r="E19" s="72" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="110"/>
+      <c r="F19" s="108"/>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="70"/>
@@ -16656,7 +16650,7 @@
       <c r="E20" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="110"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="70"/>
@@ -16672,7 +16666,7 @@
       <c r="E21" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="70"/>
@@ -16688,7 +16682,7 @@
       <c r="E22" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="70"/>
@@ -16704,7 +16698,7 @@
       <c r="E23" s="72" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="110"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="70"/>
@@ -16720,7 +16714,7 @@
       <c r="E24" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="110"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="70"/>
@@ -16736,7 +16730,7 @@
       <c r="E25" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="111"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="40" t="s">
@@ -18593,7 +18587,7 @@
       <c r="E141" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="109"/>
+      <c r="F141" s="107"/>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B142" s="71" t="s">
@@ -18608,7 +18602,7 @@
       <c r="E142" s="72" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="112"/>
+      <c r="F142" s="110"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="71" t="s">
@@ -18623,7 +18617,7 @@
       <c r="E143" s="72" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="113"/>
+      <c r="F143" s="111"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="40" t="s">
@@ -19861,7 +19855,7 @@
       <c r="E219" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="109"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B220" s="71" t="s">
@@ -19876,7 +19870,7 @@
       <c r="E220" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="108"/>
     </row>
     <row r="221" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B221" s="71" t="s">
@@ -19891,7 +19885,7 @@
       <c r="E221" s="72" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="108"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="71" t="s">
@@ -19906,7 +19900,7 @@
       <c r="E222" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="108"/>
     </row>
     <row r="223" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="71" t="s">
@@ -19921,7 +19915,7 @@
       <c r="E223" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="108"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="71" t="s">
@@ -19936,7 +19930,7 @@
       <c r="E224" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="108"/>
     </row>
     <row r="225" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B225" s="71" t="s">
@@ -19951,7 +19945,7 @@
       <c r="E225" s="72" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="110"/>
+      <c r="F225" s="108"/>
     </row>
     <row r="226" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B226" s="71" t="s">
@@ -19966,7 +19960,7 @@
       <c r="E226" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="111"/>
+      <c r="F226" s="109"/>
     </row>
     <row r="227" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B227" s="71" t="s">
@@ -20467,7 +20461,7 @@
       <c r="E11" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="106" t="s">
+      <c r="F11" s="104" t="s">
         <v>1049</v>
       </c>
     </row>
@@ -20484,7 +20478,7 @@
       <c r="E12" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="107"/>
+      <c r="F12" s="105"/>
     </row>
     <row r="13" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
@@ -20499,7 +20493,7 @@
       <c r="E13" s="12" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="107"/>
+      <c r="F13" s="105"/>
     </row>
     <row r="14" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
@@ -20514,7 +20508,7 @@
       <c r="E14" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="107"/>
+      <c r="F14" s="105"/>
     </row>
     <row r="15" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
@@ -20529,7 +20523,7 @@
       <c r="E15" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="107"/>
+      <c r="F15" s="105"/>
     </row>
     <row r="16" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
@@ -20544,7 +20538,7 @@
       <c r="E16" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="107"/>
+      <c r="F16" s="105"/>
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
@@ -20559,7 +20553,7 @@
       <c r="E17" s="12" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="107"/>
+      <c r="F17" s="105"/>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
@@ -20574,7 +20568,7 @@
       <c r="E18" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="107"/>
+      <c r="F18" s="105"/>
     </row>
     <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
@@ -20589,7 +20583,7 @@
       <c r="E19" s="12" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="107"/>
+      <c r="F19" s="105"/>
     </row>
     <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
@@ -20604,7 +20598,7 @@
       <c r="E20" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="107"/>
+      <c r="F20" s="105"/>
     </row>
     <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
@@ -20619,7 +20613,7 @@
       <c r="E21" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="107"/>
+      <c r="F21" s="105"/>
     </row>
     <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
@@ -20634,7 +20628,7 @@
       <c r="E22" s="12" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="107"/>
+      <c r="F22" s="105"/>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
@@ -20649,7 +20643,7 @@
       <c r="E23" s="12" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="107"/>
+      <c r="F23" s="105"/>
     </row>
     <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
@@ -20664,7 +20658,7 @@
       <c r="E24" s="12" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="107"/>
+      <c r="F24" s="105"/>
     </row>
     <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
@@ -20679,7 +20673,7 @@
       <c r="E25" s="12" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="108"/>
+      <c r="F25" s="106"/>
     </row>
     <row r="26" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="40" t="s">
@@ -22535,7 +22529,7 @@
       <c r="E141" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="109"/>
+      <c r="F141" s="107"/>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B142" s="71" t="s">
@@ -22550,7 +22544,7 @@
       <c r="E142" s="72" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="112"/>
+      <c r="F142" s="110"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="71" t="s">
@@ -22565,7 +22559,7 @@
       <c r="E143" s="72" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="113"/>
+      <c r="F143" s="111"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="71" t="s">
@@ -23801,7 +23795,7 @@
       <c r="E219" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="109"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B220" s="71" t="s">
@@ -23816,7 +23810,7 @@
       <c r="E220" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="108"/>
     </row>
     <row r="221" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B221" s="71" t="s">
@@ -23831,7 +23825,7 @@
       <c r="E221" s="72" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="108"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="71" t="s">
@@ -23846,7 +23840,7 @@
       <c r="E222" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="108"/>
     </row>
     <row r="223" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="71" t="s">
@@ -23861,7 +23855,7 @@
       <c r="E223" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="108"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="71" t="s">
@@ -23876,7 +23870,7 @@
       <c r="E224" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="108"/>
     </row>
     <row r="225" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B225" s="71" t="s">
@@ -23891,7 +23885,7 @@
       <c r="E225" s="72" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="110"/>
+      <c r="F225" s="108"/>
     </row>
     <row r="226" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B226" s="71" t="s">
@@ -23906,7 +23900,7 @@
       <c r="E226" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="111"/>
+      <c r="F226" s="109"/>
     </row>
     <row r="227" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B227" s="71" t="s">
@@ -24393,7 +24387,7 @@
       <c r="E11" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="2:24" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="71" t="s">
@@ -24408,7 +24402,7 @@
       <c r="E12" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="71" t="s">
@@ -24423,7 +24417,7 @@
       <c r="E13" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B14" s="71" t="s">
@@ -24438,7 +24432,7 @@
       <c r="E14" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="110"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B15" s="71" t="s">
@@ -24453,7 +24447,7 @@
       <c r="E15" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="110"/>
+      <c r="F15" s="108"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B16" s="71" t="s">
@@ -24468,7 +24462,7 @@
       <c r="E16" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="108"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="71" t="s">
@@ -24483,7 +24477,7 @@
       <c r="E17" s="72" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="71" t="s">
@@ -24498,7 +24492,7 @@
       <c r="E18" s="72" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="71" t="s">
@@ -24513,7 +24507,7 @@
       <c r="E19" s="72" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="110"/>
+      <c r="F19" s="108"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="71" t="s">
@@ -24528,7 +24522,7 @@
       <c r="E20" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="110"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="71" t="s">
@@ -24543,7 +24537,7 @@
       <c r="E21" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="71" t="s">
@@ -24558,7 +24552,7 @@
       <c r="E22" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="71" t="s">
@@ -24573,7 +24567,7 @@
       <c r="E23" s="72" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="110"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="71" t="s">
@@ -24588,7 +24582,7 @@
       <c r="E24" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="110"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="71" t="s">
@@ -24603,7 +24597,7 @@
       <c r="E25" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="111"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="40" t="s">
@@ -25298,7 +25292,7 @@
       <c r="E68" s="12" t="s">
         <v>672</v>
       </c>
-      <c r="F68" s="114" t="s">
+      <c r="F68" s="112" t="s">
         <v>1050</v>
       </c>
     </row>
@@ -25315,7 +25309,7 @@
       <c r="E69" s="12" t="s">
         <v>675</v>
       </c>
-      <c r="F69" s="115"/>
+      <c r="F69" s="113"/>
     </row>
     <row r="70" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B70" s="11" t="s">
@@ -25330,7 +25324,7 @@
       <c r="E70" s="12" t="s">
         <v>678</v>
       </c>
-      <c r="F70" s="116"/>
+      <c r="F70" s="114"/>
     </row>
     <row r="71" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B71" s="71" t="s">
@@ -26461,7 +26455,7 @@
       <c r="E141" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="109"/>
+      <c r="F141" s="107"/>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B142" s="71" t="s">
@@ -26476,7 +26470,7 @@
       <c r="E142" s="72" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="112"/>
+      <c r="F142" s="110"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="71" t="s">
@@ -26491,7 +26485,7 @@
       <c r="E143" s="72" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="113"/>
+      <c r="F143" s="111"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="71" t="s">
@@ -27727,7 +27721,7 @@
       <c r="E219" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="109"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B220" s="71" t="s">
@@ -27742,7 +27736,7 @@
       <c r="E220" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="108"/>
     </row>
     <row r="221" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B221" s="71" t="s">
@@ -27757,7 +27751,7 @@
       <c r="E221" s="72" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="108"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="71" t="s">
@@ -27772,7 +27766,7 @@
       <c r="E222" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="108"/>
     </row>
     <row r="223" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="71" t="s">
@@ -27787,7 +27781,7 @@
       <c r="E223" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="108"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="71" t="s">
@@ -27802,7 +27796,7 @@
       <c r="E224" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="108"/>
     </row>
     <row r="225" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B225" s="71" t="s">
@@ -27817,7 +27811,7 @@
       <c r="E225" s="72" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="110"/>
+      <c r="F225" s="108"/>
     </row>
     <row r="226" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B226" s="71" t="s">
@@ -27832,7 +27826,7 @@
       <c r="E226" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="111"/>
+      <c r="F226" s="109"/>
     </row>
     <row r="227" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B227" s="71" t="s">
@@ -28320,7 +28314,7 @@
       <c r="E11" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="2:24" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="71" t="s">
@@ -28335,7 +28329,7 @@
       <c r="E12" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="71" t="s">
@@ -28350,7 +28344,7 @@
       <c r="E13" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="71" t="s">
@@ -28365,7 +28359,7 @@
       <c r="E14" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="110"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="71" t="s">
@@ -28380,7 +28374,7 @@
       <c r="E15" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="110"/>
+      <c r="F15" s="108"/>
     </row>
     <row r="16" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="71" t="s">
@@ -28395,7 +28389,7 @@
       <c r="E16" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="108"/>
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="71" t="s">
@@ -28410,7 +28404,7 @@
       <c r="E17" s="72" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="71" t="s">
@@ -28425,7 +28419,7 @@
       <c r="E18" s="72" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="71" t="s">
@@ -28440,7 +28434,7 @@
       <c r="E19" s="72" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="110"/>
+      <c r="F19" s="108"/>
     </row>
     <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="71" t="s">
@@ -28455,7 +28449,7 @@
       <c r="E20" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="110"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="71" t="s">
@@ -28470,7 +28464,7 @@
       <c r="E21" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="71" t="s">
@@ -28485,7 +28479,7 @@
       <c r="E22" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="71" t="s">
@@ -28500,7 +28494,7 @@
       <c r="E23" s="72" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="110"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="71" t="s">
@@ -28515,7 +28509,7 @@
       <c r="E24" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="110"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="71" t="s">
@@ -28530,7 +28524,7 @@
       <c r="E25" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="111"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="71" t="s">
@@ -30388,7 +30382,7 @@
       <c r="E141" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="109"/>
+      <c r="F141" s="107"/>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B142" s="71" t="s">
@@ -30403,7 +30397,7 @@
       <c r="E142" s="72" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="112"/>
+      <c r="F142" s="110"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="71" t="s">
@@ -30418,7 +30412,7 @@
       <c r="E143" s="72" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="113"/>
+      <c r="F143" s="111"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="71" t="s">
@@ -31654,7 +31648,7 @@
       <c r="E219" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="109"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B220" s="71" t="s">
@@ -31669,7 +31663,7 @@
       <c r="E220" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="108"/>
     </row>
     <row r="221" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B221" s="71" t="s">
@@ -31684,7 +31678,7 @@
       <c r="E221" s="72" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="108"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="71" t="s">
@@ -31699,7 +31693,7 @@
       <c r="E222" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="108"/>
     </row>
     <row r="223" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="71" t="s">
@@ -31714,7 +31708,7 @@
       <c r="E223" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="108"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="71" t="s">
@@ -31729,7 +31723,7 @@
       <c r="E224" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="108"/>
     </row>
     <row r="225" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B225" s="71" t="s">
@@ -31744,7 +31738,7 @@
       <c r="E225" s="72" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="110"/>
+      <c r="F225" s="108"/>
     </row>
     <row r="226" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B226" s="71" t="s">
@@ -31759,7 +31753,7 @@
       <c r="E226" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="111"/>
+      <c r="F226" s="109"/>
     </row>
     <row r="227" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B227" s="71" t="s">
@@ -32246,7 +32240,7 @@
       <c r="E11" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="2:24" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="71" t="s">
@@ -32261,7 +32255,7 @@
       <c r="E12" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="71" t="s">
@@ -32276,7 +32270,7 @@
       <c r="E13" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="71" t="s">
@@ -32291,7 +32285,7 @@
       <c r="E14" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="110"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="71" t="s">
@@ -32306,7 +32300,7 @@
       <c r="E15" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="110"/>
+      <c r="F15" s="108"/>
     </row>
     <row r="16" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="71" t="s">
@@ -32321,7 +32315,7 @@
       <c r="E16" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="108"/>
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="71" t="s">
@@ -32336,7 +32330,7 @@
       <c r="E17" s="72" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="71" t="s">
@@ -32351,7 +32345,7 @@
       <c r="E18" s="72" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="71" t="s">
@@ -32366,7 +32360,7 @@
       <c r="E19" s="72" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="110"/>
+      <c r="F19" s="108"/>
     </row>
     <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="71" t="s">
@@ -32381,7 +32375,7 @@
       <c r="E20" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="110"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="71" t="s">
@@ -32396,7 +32390,7 @@
       <c r="E21" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="71" t="s">
@@ -32411,7 +32405,7 @@
       <c r="E22" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="71" t="s">
@@ -32426,7 +32420,7 @@
       <c r="E23" s="72" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="110"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="71" t="s">
@@ -32441,7 +32435,7 @@
       <c r="E24" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="110"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="71" t="s">
@@ -32456,7 +32450,7 @@
       <c r="E25" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="111"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="71" t="s">
@@ -34312,7 +34306,7 @@
       <c r="E141" s="12" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="106" t="s">
+      <c r="F141" s="104" t="s">
         <v>1060</v>
       </c>
     </row>
@@ -34329,7 +34323,7 @@
       <c r="E142" s="12" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="117"/>
+      <c r="F142" s="115"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="11" t="s">
@@ -34344,7 +34338,7 @@
       <c r="E143" s="12" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="118"/>
+      <c r="F143" s="116"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="40" t="s">
@@ -35653,7 +35647,7 @@
       <c r="E219" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="109"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A220" s="70"/>
@@ -35669,7 +35663,7 @@
       <c r="E220" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="108"/>
     </row>
     <row r="221" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A221" s="70"/>
@@ -35685,7 +35679,7 @@
       <c r="E221" s="72" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="108"/>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222" s="70"/>
@@ -35701,7 +35695,7 @@
       <c r="E222" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="108"/>
     </row>
     <row r="223" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223" s="70"/>
@@ -35717,7 +35711,7 @@
       <c r="E223" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="108"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224" s="70"/>
@@ -35733,7 +35727,7 @@
       <c r="E224" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="108"/>
     </row>
     <row r="225" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A225" s="70"/>
@@ -35749,7 +35743,7 @@
       <c r="E225" s="72" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="110"/>
+      <c r="F225" s="108"/>
     </row>
     <row r="226" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A226" s="70"/>
@@ -35765,7 +35759,7 @@
       <c r="E226" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="111"/>
+      <c r="F226" s="109"/>
     </row>
     <row r="227" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="70"/>
@@ -36276,7 +36270,7 @@
       <c r="E11" s="72" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="109"/>
+      <c r="F11" s="107"/>
     </row>
     <row r="12" spans="2:24" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="71" t="s">
@@ -36291,7 +36285,7 @@
       <c r="E12" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="F12" s="110"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="71" t="s">
@@ -36306,7 +36300,7 @@
       <c r="E13" s="72" t="s">
         <v>554</v>
       </c>
-      <c r="F13" s="110"/>
+      <c r="F13" s="108"/>
     </row>
     <row r="14" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="71" t="s">
@@ -36321,7 +36315,7 @@
       <c r="E14" s="72" t="s">
         <v>556</v>
       </c>
-      <c r="F14" s="110"/>
+      <c r="F14" s="108"/>
     </row>
     <row r="15" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="71" t="s">
@@ -36336,7 +36330,7 @@
       <c r="E15" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F15" s="110"/>
+      <c r="F15" s="108"/>
     </row>
     <row r="16" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="71" t="s">
@@ -36351,7 +36345,7 @@
       <c r="E16" s="72" t="s">
         <v>558</v>
       </c>
-      <c r="F16" s="110"/>
+      <c r="F16" s="108"/>
     </row>
     <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="71" t="s">
@@ -36366,7 +36360,7 @@
       <c r="E17" s="72" t="s">
         <v>561</v>
       </c>
-      <c r="F17" s="110"/>
+      <c r="F17" s="108"/>
     </row>
     <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="71" t="s">
@@ -36381,7 +36375,7 @@
       <c r="E18" s="72" t="s">
         <v>563</v>
       </c>
-      <c r="F18" s="110"/>
+      <c r="F18" s="108"/>
     </row>
     <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="71" t="s">
@@ -36396,7 +36390,7 @@
       <c r="E19" s="72" t="s">
         <v>1037</v>
       </c>
-      <c r="F19" s="110"/>
+      <c r="F19" s="108"/>
     </row>
     <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="71" t="s">
@@ -36411,7 +36405,7 @@
       <c r="E20" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F20" s="110"/>
+      <c r="F20" s="108"/>
     </row>
     <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="71" t="s">
@@ -36426,7 +36420,7 @@
       <c r="E21" s="72" t="s">
         <v>567</v>
       </c>
-      <c r="F21" s="110"/>
+      <c r="F21" s="108"/>
     </row>
     <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="71" t="s">
@@ -36441,7 +36435,7 @@
       <c r="E22" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="110"/>
+      <c r="F22" s="108"/>
     </row>
     <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="71" t="s">
@@ -36456,7 +36450,7 @@
       <c r="E23" s="72" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="110"/>
+      <c r="F23" s="108"/>
     </row>
     <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="71" t="s">
@@ -36471,7 +36465,7 @@
       <c r="E24" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="F24" s="110"/>
+      <c r="F24" s="108"/>
     </row>
     <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="71" t="s">
@@ -36486,7 +36480,7 @@
       <c r="E25" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="F25" s="111"/>
+      <c r="F25" s="109"/>
     </row>
     <row r="26" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" s="71" t="s">
@@ -38342,7 +38336,7 @@
       <c r="E141" s="72" t="s">
         <v>827</v>
       </c>
-      <c r="F141" s="109"/>
+      <c r="F141" s="107"/>
     </row>
     <row r="142" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B142" s="71" t="s">
@@ -38357,7 +38351,7 @@
       <c r="E142" s="72" t="s">
         <v>1039</v>
       </c>
-      <c r="F142" s="112"/>
+      <c r="F142" s="110"/>
     </row>
     <row r="143" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B143" s="71" t="s">
@@ -38372,7 +38366,7 @@
       <c r="E143" s="72" t="s">
         <v>832</v>
       </c>
-      <c r="F143" s="113"/>
+      <c r="F143" s="111"/>
     </row>
     <row r="144" spans="2:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B144" s="71" t="s">
@@ -38471,7 +38465,7 @@
       <c r="E148" s="12" t="s">
         <v>1040</v>
       </c>
-      <c r="F148" s="119" t="s">
+      <c r="F148" s="117" t="s">
         <v>1052</v>
       </c>
     </row>
@@ -38488,7 +38482,7 @@
       <c r="E149" s="12" t="s">
         <v>848</v>
       </c>
-      <c r="F149" s="120"/>
+      <c r="F149" s="118"/>
     </row>
     <row r="150" spans="2:24" s="44" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B150" s="60" t="s">
@@ -38503,7 +38497,7 @@
       <c r="E150" s="62" t="s">
         <v>851</v>
       </c>
-      <c r="F150" s="120"/>
+      <c r="F150" s="118"/>
       <c r="G150" s="31"/>
       <c r="H150" s="31"/>
       <c r="I150" s="31"/>
@@ -38536,7 +38530,7 @@
       <c r="E151" s="12" t="s">
         <v>848</v>
       </c>
-      <c r="F151" s="121"/>
+      <c r="F151" s="119"/>
     </row>
     <row r="152" spans="2:24" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B152" s="40" t="s">
@@ -39610,7 +39604,7 @@
       <c r="E219" s="72" t="s">
         <v>994</v>
       </c>
-      <c r="F219" s="109"/>
+      <c r="F219" s="107"/>
     </row>
     <row r="220" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B220" s="71" t="s">
@@ -39625,7 +39619,7 @@
       <c r="E220" s="72" t="s">
         <v>580</v>
       </c>
-      <c r="F220" s="110"/>
+      <c r="F220" s="108"/>
     </row>
     <row r="221" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B221" s="71" t="s">
@@ -39640,7 +39634,7 @@
       <c r="E221" s="72" t="s">
         <v>1041</v>
       </c>
-      <c r="F221" s="110"/>
+      <c r="F221" s="108"/>
     </row>
     <row r="222" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B222" s="71" t="s">
@@ -39655,7 +39649,7 @@
       <c r="E222" s="72" t="s">
         <v>537</v>
       </c>
-      <c r="F222" s="110"/>
+      <c r="F222" s="108"/>
     </row>
     <row r="223" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B223" s="71" t="s">
@@ -39670,7 +39664,7 @@
       <c r="E223" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="F223" s="110"/>
+      <c r="F223" s="108"/>
     </row>
     <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="71" t="s">
@@ -39685,7 +39679,7 @@
       <c r="E224" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="F224" s="110"/>
+      <c r="F224" s="108"/>
     </row>
     <row r="225" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B225" s="71" t="s">
@@ -39700,7 +39694,7 @@
       <c r="E225" s="72" t="s">
         <v>592</v>
       </c>
-      <c r="F225" s="110"/>
+      <c r="F225" s="108"/>
     </row>
     <row r="226" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B226" s="71" t="s">
@@ -39715,7 +39709,7 @@
       <c r="E226" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="F226" s="111"/>
+      <c r="F226" s="109"/>
     </row>
     <row r="227" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B227" s="71" t="s">
@@ -40703,7 +40697,7 @@
       <c r="E43" s="56" t="s">
         <v>617</v>
       </c>
-      <c r="F43" s="122" t="s">
+      <c r="F43" s="120" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -40720,7 +40714,7 @@
       <c r="E44" s="56" t="s">
         <v>619</v>
       </c>
-      <c r="F44" s="123"/>
+      <c r="F44" s="121"/>
     </row>
     <row r="45" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B45" s="55" t="s">
@@ -40735,7 +40729,7 @@
       <c r="E45" s="56" t="s">
         <v>1042</v>
       </c>
-      <c r="F45" s="123"/>
+      <c r="F45" s="121"/>
     </row>
     <row r="46" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B46" s="55" t="s">
@@ -40750,7 +40744,7 @@
       <c r="E46" s="56" t="s">
         <v>625</v>
       </c>
-      <c r="F46" s="123"/>
+      <c r="F46" s="121"/>
     </row>
     <row r="47" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B47" s="55" t="s">
@@ -40765,7 +40759,7 @@
       <c r="E47" s="56" t="s">
         <v>628</v>
       </c>
-      <c r="F47" s="124"/>
+      <c r="F47" s="122"/>
     </row>
     <row r="48" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B48" s="40" t="s">
@@ -43934,7 +43928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3477427-6C09-4E3B-AC1B-6160A9796666}">
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -44399,7 +44393,7 @@
       <c r="D28" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="92" t="s">
+      <c r="E28" s="90" t="s">
         <v>1053</v>
       </c>
     </row>
@@ -44416,7 +44410,7 @@
       <c r="D29" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="93"/>
+      <c r="E29" s="91"/>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="27" t="s">
@@ -44431,7 +44425,7 @@
       <c r="D30" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="93"/>
+      <c r="E30" s="91"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
@@ -44446,7 +44440,7 @@
       <c r="D31" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="93"/>
+      <c r="E31" s="91"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
@@ -44461,7 +44455,7 @@
       <c r="D32" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="94"/>
+      <c r="E32" s="92"/>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
@@ -44628,61 +44622,61 @@
       <c r="E42" s="22"/>
     </row>
     <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="91" t="s">
+      <c r="C43" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>116</v>
       </c>
       <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B44" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="91" t="s">
+      <c r="B44" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>118</v>
       </c>
       <c r="E44" s="22"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="91" t="s">
+      <c r="B45" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="21" t="s">
         <v>120</v>
       </c>
       <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="91" t="s">
+      <c r="B46" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="21" t="s">
         <v>122</v>
       </c>
       <c r="E46" s="22"/>
@@ -44946,7 +44940,7 @@
       <c r="D63" s="64" t="s">
         <v>159</v>
       </c>
-      <c r="E63" s="95"/>
+      <c r="E63" s="93"/>
     </row>
     <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="63" t="s">
@@ -44961,7 +44955,7 @@
       <c r="D64" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="E64" s="96"/>
+      <c r="E64" s="94"/>
     </row>
     <row r="65" spans="1:5" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="63" t="s">
@@ -44976,7 +44970,7 @@
       <c r="D65" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="96"/>
+      <c r="E65" s="94"/>
     </row>
     <row r="66" spans="1:5" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="63" t="s">
@@ -44991,7 +44985,7 @@
       <c r="D66" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="97"/>
+      <c r="E66" s="95"/>
     </row>
     <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="63" t="s">
@@ -50196,7 +50190,7 @@
       <c r="D169" s="39" t="s">
         <v>397</v>
       </c>
-      <c r="E169" s="125" t="s">
+      <c r="E169" s="123" t="s">
         <v>522</v>
       </c>
     </row>
@@ -50213,7 +50207,7 @@
       <c r="D170" s="39" t="s">
         <v>399</v>
       </c>
-      <c r="E170" s="126"/>
+      <c r="E170" s="124"/>
     </row>
     <row r="171" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A171" s="38" t="s">
@@ -50228,7 +50222,7 @@
       <c r="D171" s="39" t="s">
         <v>523</v>
       </c>
-      <c r="E171" s="126"/>
+      <c r="E171" s="124"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="38" t="s">
@@ -50243,7 +50237,7 @@
       <c r="D172" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="E172" s="126"/>
+      <c r="E172" s="124"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="38" t="s">
@@ -50258,7 +50252,7 @@
       <c r="D173" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="E173" s="127"/>
+      <c r="E173" s="125"/>
     </row>
     <row r="174" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="20" t="s">
@@ -51022,7 +51016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E51970-45E7-423A-A6F9-1C957942FC2A}">
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -51487,7 +51481,7 @@
       <c r="D28" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="95"/>
+      <c r="E28" s="93"/>
     </row>
     <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="63" t="s">
@@ -51502,7 +51496,7 @@
       <c r="D29" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="96"/>
+      <c r="E29" s="94"/>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="63" t="s">
@@ -51517,7 +51511,7 @@
       <c r="D30" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="96"/>
+      <c r="E30" s="94"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="63" t="s">
@@ -51532,7 +51526,7 @@
       <c r="D31" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="96"/>
+      <c r="E31" s="94"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="63" t="s">
@@ -51547,7 +51541,7 @@
       <c r="D32" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="97"/>
+      <c r="E32" s="95"/>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
@@ -51726,7 +51720,7 @@
       <c r="D43" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="E43" s="98" t="s">
+      <c r="E43" s="96" t="s">
         <v>1062</v>
       </c>
     </row>
@@ -51743,7 +51737,7 @@
       <c r="D44" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="E44" s="99"/>
+      <c r="E44" s="97"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="38" t="s">
@@ -51758,7 +51752,7 @@
       <c r="D45" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="E45" s="99"/>
+      <c r="E45" s="97"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="38" t="s">
@@ -51773,7 +51767,7 @@
       <c r="D46" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="100"/>
+      <c r="E46" s="98"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
@@ -54990,7 +54984,7 @@
       <c r="D28" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="101" t="s">
+      <c r="E28" s="99" t="s">
         <v>1055</v>
       </c>
     </row>
@@ -55007,7 +55001,7 @@
       <c r="D29" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="102"/>
+      <c r="E29" s="100"/>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
@@ -55022,7 +55016,7 @@
       <c r="D30" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="102"/>
+      <c r="E30" s="100"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="38" t="s">
@@ -55037,7 +55031,7 @@
       <c r="D31" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="102"/>
+      <c r="E31" s="100"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
@@ -55052,7 +55046,7 @@
       <c r="D32" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="103"/>
+      <c r="E32" s="101"/>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
@@ -61991,7 +61985,7 @@
       <c r="D28" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="95"/>
+      <c r="E28" s="93"/>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="63" t="s">
@@ -62006,7 +62000,7 @@
       <c r="D29" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="96"/>
+      <c r="E29" s="94"/>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="63" t="s">
@@ -62021,7 +62015,7 @@
       <c r="D30" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="96"/>
+      <c r="E30" s="94"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="63" t="s">
@@ -62036,7 +62030,7 @@
       <c r="D31" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="96"/>
+      <c r="E31" s="94"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="63" t="s">
@@ -62051,7 +62045,7 @@
       <c r="D32" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="97"/>
+      <c r="E32" s="95"/>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="63" t="s">
@@ -66038,7 +66032,7 @@
       <c r="D63" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="E63" s="98" t="s">
+      <c r="E63" s="96" t="s">
         <v>1057</v>
       </c>
     </row>
@@ -66055,7 +66049,7 @@
       <c r="D64" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E64" s="99"/>
+      <c r="E64" s="97"/>
     </row>
     <row r="65" spans="1:5" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A65" s="38" t="s">
@@ -66070,7 +66064,7 @@
       <c r="D65" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="99"/>
+      <c r="E65" s="97"/>
     </row>
     <row r="66" spans="1:5" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="38" t="s">
@@ -66085,7 +66079,7 @@
       <c r="D66" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="99"/>
+      <c r="E66" s="97"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="38" t="s">
@@ -66100,7 +66094,7 @@
       <c r="D67" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="100"/>
+      <c r="E67" s="98"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
@@ -70815,7 +70809,7 @@
       <c r="D144" s="39" t="s">
         <v>329</v>
       </c>
-      <c r="E144" s="98" t="s">
+      <c r="E144" s="96" t="s">
         <v>1058</v>
       </c>
     </row>
@@ -70832,7 +70826,7 @@
       <c r="D145" s="39" t="s">
         <v>339</v>
       </c>
-      <c r="E145" s="104"/>
+      <c r="E145" s="102"/>
     </row>
     <row r="146" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A146" s="38" t="s">
@@ -70847,7 +70841,7 @@
       <c r="D146" s="39" t="s">
         <v>342</v>
       </c>
-      <c r="E146" s="104"/>
+      <c r="E146" s="102"/>
     </row>
     <row r="147" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="38" t="s">
@@ -70862,7 +70856,7 @@
       <c r="D147" s="39" t="s">
         <v>345</v>
       </c>
-      <c r="E147" s="104"/>
+      <c r="E147" s="102"/>
     </row>
     <row r="148" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="38" t="s">
@@ -70877,7 +70871,7 @@
       <c r="D148" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="E148" s="105"/>
+      <c r="E148" s="103"/>
     </row>
     <row r="149" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A149" s="20" t="s">
@@ -71194,76 +71188,76 @@
       <c r="E168" s="22"/>
     </row>
     <row r="169" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A169" s="90" t="s">
+      <c r="A169" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="B169" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="C169" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="D169" s="91" t="s">
+      <c r="B169" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C169" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D169" s="21" t="s">
         <v>397</v>
       </c>
       <c r="E169" s="22"/>
     </row>
     <row r="170" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A170" s="90" t="s">
+      <c r="A170" s="20" t="s">
         <v>398</v>
       </c>
-      <c r="B170" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C170" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D170" s="91" t="s">
+      <c r="B170" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D170" s="21" t="s">
         <v>399</v>
       </c>
       <c r="E170" s="22"/>
     </row>
     <row r="171" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A171" s="90" t="s">
+      <c r="A171" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="B171" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C171" s="91" t="s">
-        <v>8</v>
-      </c>
-      <c r="D171" s="91" t="s">
+      <c r="B171" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C171" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D171" s="21" t="s">
         <v>523</v>
       </c>
       <c r="E171" s="22"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A172" s="90" t="s">
+      <c r="A172" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="B172" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="C172" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="D172" s="91" t="s">
+      <c r="B172" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D172" s="21" t="s">
         <v>65</v>
       </c>
       <c r="E172" s="22"/>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A173" s="90" t="s">
+      <c r="A173" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="B173" s="91" t="s">
-        <v>40</v>
-      </c>
-      <c r="C173" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="D173" s="91" t="s">
+      <c r="B173" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D173" s="21" t="s">
         <v>67</v>
       </c>
       <c r="E173" s="22"/>
@@ -74601,7 +74595,7 @@
       <c r="D162" s="39" t="s">
         <v>379</v>
       </c>
-      <c r="E162" s="101" t="s">
+      <c r="E162" s="99" t="s">
         <v>524</v>
       </c>
     </row>
@@ -74618,7 +74612,7 @@
       <c r="D163" s="39" t="s">
         <v>525</v>
       </c>
-      <c r="E163" s="102"/>
+      <c r="E163" s="100"/>
     </row>
     <row r="164" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A164" s="38" t="s">
@@ -74633,7 +74627,7 @@
       <c r="D164" s="39" t="s">
         <v>526</v>
       </c>
-      <c r="E164" s="102"/>
+      <c r="E164" s="100"/>
     </row>
     <row r="165" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="38" t="s">
@@ -74648,7 +74642,7 @@
       <c r="D165" s="39" t="s">
         <v>387</v>
       </c>
-      <c r="E165" s="102"/>
+      <c r="E165" s="100"/>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="38" t="s">
@@ -74663,7 +74657,7 @@
       <c r="D166" s="39" t="s">
         <v>390</v>
       </c>
-      <c r="E166" s="103"/>
+      <c r="E166" s="101"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="20" t="s">
@@ -75754,6 +75748,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d04b37e-0497-498c-96f6-8855740e5edb">
@@ -75761,15 +75764,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -75792,6 +75786,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51A983D-5463-4E4A-8B75-1C405A420DB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99C0AEB7-C55A-461D-A0CE-4337A3223303}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -75806,12 +75808,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F51A983D-5463-4E4A-8B75-1C405A420DB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>